<commit_message>
Corretto Piccolo Errore Foglio Excel
</commit_message>
<xml_diff>
--- a/Interfaccia Gara PC/Sistema Interfaccia 24_05/Elenco Piloti Al 23_05.xlsx
+++ b/Interfaccia Gara PC/Sistema Interfaccia 24_05/Elenco Piloti Al 23_05.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\Documents\GitHub\Sistema_Pylon\Interfaccia Gara PC\Sistema Interfaccia 14_05_23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\Documents\GitHub\Sistema_Pylon\Interfaccia Gara PC\Sistema Interfaccia 24_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129ACE59-5582-40B5-B88A-F2BCD0E28FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C0F113-D625-4BEA-B0E6-526827BC381E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$40</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -635,21 +635,6 @@
   </si>
   <si>
     <t>wim_lentjes@hotmaol.com</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Fehling</t>
-  </si>
-  <si>
-    <t>Ricki</t>
-  </si>
-  <si>
-    <t>Racker</t>
-  </si>
-  <si>
-    <t>evangelion5154@hotmail.com</t>
   </si>
   <si>
     <t>Massimo</t>
@@ -679,11 +664,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1051,10 +1038,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A41"/>
+      <selection activeCell="A39" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1051,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1185,7 +1172,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A41" si="0">A3+1</f>
+        <f t="shared" ref="A4:A40" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -2395,10 +2382,10 @@
         <v>183</v>
       </c>
       <c r="D34" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E34" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F34" t="s">
         <v>83</v>
@@ -2635,7 +2622,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2647,68 +2634,23 @@
         <v>200</v>
       </c>
       <c r="D40" t="s">
+        <v>182</v>
+      </c>
+      <c r="E40" t="s">
+        <v>183</v>
+      </c>
+      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" t="s">
         <v>201</v>
       </c>
-      <c r="E40" t="s">
-        <v>202</v>
-      </c>
-      <c r="F40" t="s">
-        <v>76</v>
-      </c>
-      <c r="G40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J40" t="s">
-        <v>70</v>
-      </c>
-      <c r="K40" t="s">
-        <v>70</v>
-      </c>
-      <c r="L40" t="s">
-        <v>35</v>
-      </c>
-      <c r="M40" t="s">
-        <v>203</v>
-      </c>
-      <c r="N40" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>204</v>
-      </c>
-      <c r="C41" t="s">
-        <v>205</v>
-      </c>
-      <c r="D41" t="s">
-        <v>182</v>
-      </c>
-      <c r="E41" t="s">
-        <v>183</v>
-      </c>
-      <c r="F41" t="s">
-        <v>83</v>
-      </c>
-      <c r="G41" t="s">
-        <v>206</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="H40" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H41" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="H1:H40" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>